<commit_message>
'added April in successful by experience'
</commit_message>
<xml_diff>
--- a/seasonal_patterns/high.xlsx
+++ b/seasonal_patterns/high.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
fixed line 476. replaced travellers size with the correct aggregation which is sum.
</commit_message>
<xml_diff>
--- a/seasonal_patterns/high.xlsx
+++ b/seasonal_patterns/high.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,13 +493,13 @@
         <v>189.81</v>
       </c>
       <c r="F2" t="n">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="G2" t="n">
         <v>1800</v>
       </c>
       <c r="H2" t="n">
-        <v>300</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="3">
@@ -557,13 +557,13 @@
         <v>49.95</v>
       </c>
       <c r="F4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G4" t="n">
         <v>400</v>
       </c>
       <c r="H4" t="n">
-        <v>300</v>
+        <v>400</v>
       </c>
     </row>
     <row r="5">
@@ -589,13 +589,13 @@
         <v>39.96</v>
       </c>
       <c r="F5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G5" t="n">
         <v>1214.473684210527</v>
       </c>
       <c r="H5" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6">
@@ -621,18 +621,18 @@
         <v>388.96</v>
       </c>
       <c r="F6" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G6" t="n">
         <v>194.6889915902719</v>
       </c>
       <c r="H6" t="n">
-        <v>266.6666666666666</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -641,30 +641,30 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>EN</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>2652.88</v>
+        <v>2037.96</v>
       </c>
       <c r="F7" t="n">
-        <v>35</v>
+        <v>204</v>
       </c>
       <c r="G7" t="n">
-        <v>397.2782484816675</v>
+        <v>973.6842105263157</v>
       </c>
       <c r="H7" t="n">
-        <v>250</v>
+        <v>973.6842105263157</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -673,7 +673,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Singapore</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -682,21 +682,21 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>47.96</v>
+        <v>61245.7</v>
       </c>
       <c r="F8" t="n">
-        <v>3</v>
+        <v>3185</v>
       </c>
       <c r="G8" t="n">
-        <v>100</v>
+        <v>242.6118195671096</v>
       </c>
       <c r="H8" t="n">
-        <v>200</v>
+        <v>205.9558117195005</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -705,7 +705,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -714,21 +714,21 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>1356</v>
+        <v>2652.88</v>
       </c>
       <c r="F9" t="n">
-        <v>32</v>
+        <v>113</v>
       </c>
       <c r="G9" t="n">
-        <v>236.8944099378882</v>
+        <v>397.2782484816675</v>
       </c>
       <c r="H9" t="n">
-        <v>357.1428571428571</v>
+        <v>351.9999999999999</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -737,25 +737,25 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>EN</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>84.05</v>
+        <v>1356</v>
       </c>
       <c r="F10" t="n">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="G10" t="n">
-        <v>-17.91992187500001</v>
+        <v>236.8944099378882</v>
       </c>
       <c r="H10" t="n">
-        <v>250</v>
+        <v>261.1111111111111</v>
       </c>
     </row>
     <row r="11">
@@ -781,13 +781,13 @@
         <v>185.76</v>
       </c>
       <c r="F11" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G11" t="n">
         <v>382.4935064935065</v>
       </c>
       <c r="H11" t="n">
-        <v>500</v>
+        <v>400</v>
       </c>
     </row>
     <row r="12">
@@ -813,13 +813,13 @@
         <v>45373.76</v>
       </c>
       <c r="F12" t="n">
-        <v>878</v>
+        <v>1782</v>
       </c>
       <c r="G12" t="n">
         <v>633.6939244440348</v>
       </c>
       <c r="H12" t="n">
-        <v>343.4343434343434</v>
+        <v>384.2391304347826</v>
       </c>
     </row>
     <row r="13">
@@ -856,7 +856,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -865,30 +865,30 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>EN</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>73.83</v>
+        <v>2213.47</v>
       </c>
       <c r="F14" t="n">
-        <v>8</v>
+        <v>92</v>
       </c>
       <c r="G14" t="n">
-        <v>824.0300375469337</v>
+        <v>415.5277622507919</v>
       </c>
       <c r="H14" t="n">
-        <v>700</v>
+        <v>228.5714285714286</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -897,30 +897,30 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>EN</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>4174.2</v>
+        <v>73.83</v>
       </c>
       <c r="F15" t="n">
-        <v>94</v>
+        <v>9</v>
       </c>
       <c r="G15" t="n">
-        <v>1305.454545454545</v>
+        <v>824.0300375469337</v>
       </c>
       <c r="H15" t="n">
-        <v>840</v>
+        <v>800</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -934,25 +934,25 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>ES</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>26678.2</v>
+        <v>4174.2</v>
       </c>
       <c r="F16" t="n">
-        <v>530</v>
+        <v>205</v>
       </c>
       <c r="G16" t="n">
-        <v>672.5757641573636</v>
+        <v>1305.454545454545</v>
       </c>
       <c r="H16" t="n">
-        <v>516.2790697674419</v>
+        <v>1181.25</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -966,25 +966,25 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>EN</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>14614.88</v>
+        <v>78870.77</v>
       </c>
       <c r="F17" t="n">
-        <v>319</v>
+        <v>4046</v>
       </c>
       <c r="G17" t="n">
-        <v>332.9590766623811</v>
+        <v>219.734137194483</v>
       </c>
       <c r="H17" t="n">
-        <v>266.6666666666666</v>
+        <v>213.4004647560031</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -998,25 +998,25 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>ES</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>1193.9</v>
+        <v>26678.2</v>
       </c>
       <c r="F18" t="n">
-        <v>24</v>
+        <v>1399</v>
       </c>
       <c r="G18" t="n">
-        <v>421.353711790393</v>
+        <v>672.5757641573636</v>
       </c>
       <c r="H18" t="n">
-        <v>300</v>
+        <v>632.4607329842931</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1025,71 +1025,71 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>EN</t>
+          <t>FR</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>2209.17</v>
+        <v>14614.88</v>
       </c>
       <c r="F19" t="n">
-        <v>29</v>
+        <v>789</v>
       </c>
       <c r="G19" t="n">
-        <v>2528.399762046401</v>
+        <v>332.9590766623811</v>
       </c>
       <c r="H19" t="n">
-        <v>314.2857142857143</v>
+        <v>333.5164835164835</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>205</v>
+        <v>22</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>June</t>
+          <t>April</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>EN</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>39.96</v>
+        <v>1193.9</v>
       </c>
       <c r="F20" t="n">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="G20" t="n">
-        <v>300</v>
+        <v>421.353711790393</v>
       </c>
       <c r="H20" t="n">
-        <v>200</v>
+        <v>390.9090909090909</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>212</v>
+        <v>28</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>June</t>
+          <t>April</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Singapore</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1098,21 +1098,21 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>73.93000000000001</v>
+        <v>2209.17</v>
       </c>
       <c r="F21" t="n">
-        <v>3</v>
+        <v>92</v>
       </c>
       <c r="G21" t="n">
-        <v>48.00800800800802</v>
+        <v>2528.399762046401</v>
       </c>
       <c r="H21" t="n">
-        <v>200</v>
+        <v>1214.285714285714</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1121,62 +1121,62 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>ES</t>
+          <t>EN</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>1083.77</v>
+        <v>39.96</v>
       </c>
       <c r="F22" t="n">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="G22" t="n">
-        <v>204.0454481694487</v>
+        <v>300</v>
       </c>
       <c r="H22" t="n">
-        <v>225</v>
+        <v>300</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>157</v>
+        <v>215</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>July</t>
+          <t>June</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>EN</t>
+          <t>ES</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>59.57</v>
+        <v>1083.77</v>
       </c>
       <c r="F23" t="n">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="G23" t="n">
-        <v>98.76543209876544</v>
+        <v>204.0454481694487</v>
       </c>
       <c r="H23" t="n">
-        <v>250</v>
+        <v>233.3333333333333</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -1185,25 +1185,25 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>EN</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>150.1</v>
+        <v>259</v>
       </c>
       <c r="F24" t="n">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="G24" t="n">
-        <v>115.351506456241</v>
+        <v>1380</v>
       </c>
       <c r="H24" t="n">
-        <v>200</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="25">
@@ -1229,13 +1229,13 @@
         <v>30.96</v>
       </c>
       <c r="F25" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G25" t="n">
         <v>209.9099099099099</v>
       </c>
       <c r="H25" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
     </row>
     <row r="26">
@@ -1261,18 +1261,18 @@
         <v>554</v>
       </c>
       <c r="F26" t="n">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="G26" t="n">
         <v>1267.901234567901</v>
       </c>
       <c r="H26" t="n">
-        <v>1000</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1281,30 +1281,30 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>3077.81</v>
+        <v>4283.9</v>
       </c>
       <c r="F27" t="n">
-        <v>50</v>
+        <v>196</v>
       </c>
       <c r="G27" t="n">
-        <v>318.3739771089906</v>
+        <v>241.8914604948124</v>
       </c>
       <c r="H27" t="n">
-        <v>257.1428571428572</v>
+        <v>216.1290322580645</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1313,94 +1313,94 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>FR</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>608.5</v>
+        <v>3077.81</v>
       </c>
       <c r="F28" t="n">
-        <v>10</v>
+        <v>136</v>
       </c>
       <c r="G28" t="n">
-        <v>305.3964023984011</v>
+        <v>318.3739771089906</v>
       </c>
       <c r="H28" t="n">
-        <v>233.3333333333333</v>
+        <v>300</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>362</v>
+        <v>64</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>September</t>
+          <t>August</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>CH</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>432.5</v>
+        <v>608.5</v>
       </c>
       <c r="F29" t="n">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="G29" t="n">
-        <v>3507.172643869892</v>
+        <v>305.3964023984011</v>
       </c>
       <c r="H29" t="n">
-        <v>400</v>
+        <v>285.7142857142857</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>384</v>
+        <v>65</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>September</t>
+          <t>August</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>EN</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>1978.1</v>
+        <v>5100.38</v>
       </c>
       <c r="F30" t="n">
-        <v>70</v>
+        <v>148</v>
       </c>
       <c r="G30" t="n">
-        <v>247.8834350433513</v>
+        <v>266.1514605483248</v>
       </c>
       <c r="H30" t="n">
-        <v>250</v>
+        <v>208.3333333333333</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>388</v>
+        <v>362</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -1409,167 +1409,167 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>CH</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>585.02</v>
+        <v>432.5</v>
       </c>
       <c r="F31" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="G31" t="n">
-        <v>132.5013909864081</v>
+        <v>3507.172643869892</v>
       </c>
       <c r="H31" t="n">
-        <v>257.1428571428572</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>325</v>
+        <v>375</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>October</t>
+          <t>September</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>EN</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>29.97</v>
+        <v>39.95</v>
       </c>
       <c r="F32" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G32" t="n">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="H32" t="n">
-        <v>200</v>
+        <v>400</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>326</v>
+        <v>384</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>October</t>
+          <t>September</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>CH</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>1763.47</v>
+        <v>1978.1</v>
       </c>
       <c r="F33" t="n">
-        <v>31</v>
+        <v>138</v>
       </c>
       <c r="G33" t="n">
-        <v>307.7387283236994</v>
+        <v>247.8834350433513</v>
       </c>
       <c r="H33" t="n">
-        <v>520</v>
+        <v>305.8823529411765</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>331</v>
+        <v>388</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>October</t>
+          <t>September</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>GR</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>322.05</v>
+        <v>585.02</v>
       </c>
       <c r="F34" t="n">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="G34" t="n">
-        <v>386.6273798730734</v>
+        <v>132.5013909864081</v>
       </c>
       <c r="H34" t="n">
-        <v>250</v>
+        <v>300</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>334</v>
+        <v>391</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>October</t>
+          <t>September</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>EN</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>3461.89</v>
+        <v>419.37</v>
       </c>
       <c r="F35" t="n">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="G35" t="n">
-        <v>344.5159219311762</v>
+        <v>324.506529000911</v>
       </c>
       <c r="H35" t="n">
-        <v>213.6363636363636</v>
+        <v>338.4615384615385</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>286</v>
+        <v>325</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>November</t>
+          <t>October</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Austria</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1578,13 +1578,13 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>97.95</v>
+        <v>29.97</v>
       </c>
       <c r="F36" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G36" t="n">
-        <v>226.8268268268268</v>
+        <v>200</v>
       </c>
       <c r="H36" t="n">
         <v>200</v>
@@ -1592,34 +1592,258 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
+        <v>326</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>October</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Greece</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>CH</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>1763.47</v>
+      </c>
+      <c r="F37" t="n">
+        <v>68</v>
+      </c>
+      <c r="G37" t="n">
+        <v>307.7387283236994</v>
+      </c>
+      <c r="H37" t="n">
+        <v>353.3333333333333</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>331</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>October</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Greece</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>GR</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>322.05</v>
+      </c>
+      <c r="F38" t="n">
+        <v>34</v>
+      </c>
+      <c r="G38" t="n">
+        <v>386.6273798730734</v>
+      </c>
+      <c r="H38" t="n">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>334</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>October</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>DE</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>3461.89</v>
+      </c>
+      <c r="F39" t="n">
+        <v>175</v>
+      </c>
+      <c r="G39" t="n">
+        <v>344.5159219311762</v>
+      </c>
+      <c r="H39" t="n">
+        <v>306.9767441860465</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>354</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>October</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>United Kingdom</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>EN</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>65.78999999999999</v>
+      </c>
+      <c r="F40" t="n">
+        <v>3</v>
+      </c>
+      <c r="G40" t="n">
+        <v>558.5585585585585</v>
+      </c>
+      <c r="H40" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>289</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>November</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>EN</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>2025.98</v>
+      </c>
+      <c r="F41" t="n">
+        <v>203</v>
+      </c>
+      <c r="G41" t="n">
+        <v>1222.354937667254</v>
+      </c>
+      <c r="H41" t="n">
+        <v>2155.555555555556</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>290</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>November</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Germany</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>EN</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>10027.37</v>
+      </c>
+      <c r="F42" t="n">
+        <v>1004</v>
+      </c>
+      <c r="G42" t="n">
+        <v>33358.02469135803</v>
+      </c>
+      <c r="H42" t="n">
+        <v>33366.66666666667</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
         <v>318</v>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="B43" t="inlineStr">
         <is>
           <t>November</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="C43" t="inlineStr">
         <is>
           <t>United States</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>EN</t>
-        </is>
-      </c>
-      <c r="E37" t="n">
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>EN</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
         <v>2237.02</v>
       </c>
-      <c r="F37" t="n">
-        <v>50</v>
-      </c>
-      <c r="G37" t="n">
+      <c r="F43" t="n">
+        <v>226</v>
+      </c>
+      <c r="G43" t="n">
         <v>604.1518461393182</v>
       </c>
-      <c r="H37" t="n">
-        <v>733.3333333333334</v>
+      <c r="H43" t="n">
+        <v>629.0322580645161</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Netherlands</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>EN</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>35.97</v>
+      </c>
+      <c r="F44" t="n">
+        <v>3</v>
+      </c>
+      <c r="G44" t="n">
+        <v>350.1877346683353</v>
+      </c>
+      <c r="H44" t="n">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>